<commit_message>
linked tables MIF - MIF_visit
</commit_message>
<xml_diff>
--- a/app/config/tables/MIF_VISIT/forms/MIF_VISIT/MIF_VISIT.xlsx
+++ b/app/config/tables/MIF_VISIT/forms/MIF_VISIT/MIF_VISIT.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C82B82-4A87-4CB2-8CB0-8EF2EE3A8AC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1245229B-031E-4005-B2C5-EC95D0DEBD50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -401,9 +401,6 @@
     <t>Data de visita</t>
   </si>
   <si>
-    <t>ASSISTENTE</t>
-  </si>
-  <si>
     <t>Assistent</t>
   </si>
   <si>
@@ -995,9 +992,6 @@
     <t>Preencher Ficha de Obito de MIF</t>
   </si>
   <si>
-    <t>data('GR') != '1' || data('PARPAD') != '2'</t>
-  </si>
-  <si>
     <t>GR_LAST</t>
   </si>
   <si>
@@ -1074,6 +1068,12 @@
   </si>
   <si>
     <t>data('ESTADOVIS') != '2' &amp;&amp; data('ESTADOVIS') !='3' &amp;&amp; data('GR_LAST') != "1"  &amp;&amp; data('PARPAD3') !='1'</t>
+  </si>
+  <si>
+    <t>ASSISTANT</t>
+  </si>
+  <si>
+    <t>data('GR') != '1' || (data('PARPAD') != '2' &amp;&amp; data('PARPAD3') != '1')</t>
   </si>
 </sst>
 </file>
@@ -1623,13 +1623,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>18</v>
@@ -1640,7 +1640,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -1656,7 +1656,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -1664,10 +1664,10 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
+        <v>244</v>
+      </c>
+      <c r="D5" t="s">
         <v>245</v>
-      </c>
-      <c r="D5" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -1683,7 +1683,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E7" t="s">
         <v>19</v>
@@ -1694,18 +1694,18 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="B8" s="17" t="s">
         <v>186</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1718,9 +1718,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F97EDFF-72E2-4781-A226-FCA8C7C63015}">
   <dimension ref="A1:L119"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G39" sqref="G39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C100" sqref="C100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1758,7 +1758,7 @@
         <v>10</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>11</v>
@@ -1767,13 +1767,13 @@
         <v>116</v>
       </c>
       <c r="J1" s="16" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="K1" s="22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
@@ -1784,7 +1784,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F3" t="s">
         <v>118</v>
@@ -1801,16 +1801,16 @@
         <v>113</v>
       </c>
       <c r="E4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F4" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="G4" t="s">
         <v>121</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>122</v>
-      </c>
-      <c r="H4" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
@@ -1831,13 +1831,13 @@
         <v>52</v>
       </c>
       <c r="F7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G7" t="s">
+        <v>124</v>
+      </c>
+      <c r="H7" t="s">
         <v>125</v>
-      </c>
-      <c r="H7" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
@@ -1845,21 +1845,21 @@
         <v>114</v>
       </c>
       <c r="C8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F9" t="s">
+        <v>126</v>
+      </c>
+      <c r="G9" t="s">
         <v>127</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>128</v>
-      </c>
-      <c r="H9" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
@@ -1867,7 +1867,7 @@
         <v>114</v>
       </c>
       <c r="C10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
@@ -1875,13 +1875,13 @@
         <v>111</v>
       </c>
       <c r="F11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
@@ -1906,7 +1906,7 @@
         <v>114</v>
       </c>
       <c r="C15" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.35">
@@ -1916,16 +1916,16 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G17" s="24" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H17" s="24" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="L17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.35">
@@ -1944,7 +1944,7 @@
         <v>114</v>
       </c>
       <c r="C21" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.35">
@@ -1955,13 +1955,13 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D23" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G23" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="H23" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.35">
@@ -1972,7 +1972,7 @@
         <v>27</v>
       </c>
       <c r="F24" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.35">
@@ -1991,7 +1991,7 @@
         <v>114</v>
       </c>
       <c r="C27" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.35">
@@ -2000,7 +2000,7 @@
         <v>114</v>
       </c>
       <c r="C28" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.35">
@@ -2011,13 +2011,13 @@
     <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B30" s="24"/>
       <c r="D30" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G30" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="H30" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.35">
@@ -2029,13 +2029,13 @@
         <v>27</v>
       </c>
       <c r="F31" t="s">
+        <v>132</v>
+      </c>
+      <c r="G31" t="s">
         <v>133</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>134</v>
-      </c>
-      <c r="H31" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.35">
@@ -2047,13 +2047,13 @@
         <v>27</v>
       </c>
       <c r="F32" t="s">
+        <v>135</v>
+      </c>
+      <c r="G32" t="s">
         <v>136</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
         <v>137</v>
-      </c>
-      <c r="H32" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.35">
@@ -2061,10 +2061,10 @@
         <v>114</v>
       </c>
       <c r="C33" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="L33" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.35">
@@ -2072,10 +2072,10 @@
         <v>115</v>
       </c>
       <c r="J34" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K34" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.35">
@@ -2095,7 +2095,7 @@
         <v>114</v>
       </c>
       <c r="C37" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.35">
@@ -2106,13 +2106,13 @@
     <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B39" s="24"/>
       <c r="D39" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G39" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="H39" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.35">
@@ -2124,13 +2124,13 @@
         <v>27</v>
       </c>
       <c r="F40" t="s">
+        <v>132</v>
+      </c>
+      <c r="G40" t="s">
         <v>133</v>
       </c>
-      <c r="G40" t="s">
+      <c r="H40" t="s">
         <v>134</v>
-      </c>
-      <c r="H40" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.35">
@@ -2142,13 +2142,13 @@
         <v>27</v>
       </c>
       <c r="F41" t="s">
+        <v>135</v>
+      </c>
+      <c r="G41" t="s">
         <v>136</v>
       </c>
-      <c r="G41" t="s">
+      <c r="H41" t="s">
         <v>137</v>
-      </c>
-      <c r="H41" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.35">
@@ -2156,10 +2156,10 @@
         <v>114</v>
       </c>
       <c r="C42" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="L42" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.35">
@@ -2167,10 +2167,10 @@
         <v>115</v>
       </c>
       <c r="J43" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K43" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.35">
@@ -2190,7 +2190,7 @@
         <v>114</v>
       </c>
       <c r="C47" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.35">
@@ -2207,13 +2207,13 @@
         <v>27</v>
       </c>
       <c r="F49" t="s">
+        <v>138</v>
+      </c>
+      <c r="G49" t="s">
         <v>139</v>
       </c>
-      <c r="G49" t="s">
+      <c r="H49" t="s">
         <v>140</v>
-      </c>
-      <c r="H49" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.35">
@@ -2233,7 +2233,7 @@
         <v>114</v>
       </c>
       <c r="C52" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.35">
@@ -2246,16 +2246,16 @@
       <c r="A54" s="27"/>
       <c r="B54" s="26"/>
       <c r="D54" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F54" t="s">
+        <v>164</v>
+      </c>
+      <c r="G54" t="s">
         <v>165</v>
       </c>
-      <c r="G54" t="s">
+      <c r="H54" t="s">
         <v>166</v>
-      </c>
-      <c r="H54" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.35">
@@ -2268,13 +2268,13 @@
         <v>70</v>
       </c>
       <c r="F55" t="s">
+        <v>142</v>
+      </c>
+      <c r="G55" t="s">
         <v>143</v>
       </c>
-      <c r="G55" t="s">
+      <c r="H55" t="s">
         <v>144</v>
-      </c>
-      <c r="H55" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.35">
@@ -2289,7 +2289,7 @@
         <v>114</v>
       </c>
       <c r="C57" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.35">
@@ -2308,13 +2308,13 @@
         <v>27</v>
       </c>
       <c r="F59" t="s">
+        <v>168</v>
+      </c>
+      <c r="G59" t="s">
         <v>169</v>
       </c>
-      <c r="G59" t="s">
-        <v>170</v>
-      </c>
       <c r="H59" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.35">
@@ -2323,42 +2323,42 @@
         <v>114</v>
       </c>
       <c r="C60" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" s="27"/>
       <c r="B61" s="5"/>
       <c r="D61" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F61" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="G61" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="H61" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" s="27"/>
       <c r="B62" s="5"/>
       <c r="D62" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E62" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="F62" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="G62" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="H62" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.35">
@@ -2376,7 +2376,7 @@
     <row r="65" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A65" s="27"/>
       <c r="B65" s="5" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="66" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.35">
@@ -2385,7 +2385,7 @@
         <v>114</v>
       </c>
       <c r="C66" s="19" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="67" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.35">
@@ -2397,22 +2397,22 @@
     <row r="68" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A68" s="27"/>
       <c r="D68" s="19" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G68" s="19" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="H68" s="19" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="69" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A69" s="27"/>
       <c r="D69" s="19" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E69" s="19" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="70" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.35">
@@ -2432,7 +2432,7 @@
         <v>114</v>
       </c>
       <c r="C73" s="28" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D73" s="28"/>
       <c r="E73" s="28"/>
@@ -2463,15 +2463,15 @@
       <c r="B75" s="28"/>
       <c r="C75" s="28"/>
       <c r="D75" s="28" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E75" s="28"/>
       <c r="F75" s="28"/>
       <c r="G75" s="28" t="s">
+        <v>286</v>
+      </c>
+      <c r="H75" s="28" t="s">
         <v>287</v>
-      </c>
-      <c r="H75" s="28" t="s">
-        <v>288</v>
       </c>
       <c r="I75" s="28"/>
       <c r="J75" s="28"/>
@@ -2482,10 +2482,10 @@
       <c r="B76" s="28"/>
       <c r="C76" s="28"/>
       <c r="D76" s="28" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E76" s="28" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F76" s="28"/>
       <c r="G76" s="28"/>
@@ -2530,7 +2530,7 @@
         <v>114</v>
       </c>
       <c r="C80" s="19" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D80" s="24"/>
       <c r="E80" s="24"/>
@@ -2561,15 +2561,15 @@
       <c r="B82" s="24"/>
       <c r="C82" s="24"/>
       <c r="D82" s="24" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E82" s="24"/>
       <c r="F82" s="24"/>
       <c r="G82" s="24" t="s">
+        <v>290</v>
+      </c>
+      <c r="H82" s="24" t="s">
         <v>291</v>
-      </c>
-      <c r="H82" s="24" t="s">
-        <v>292</v>
       </c>
       <c r="I82" s="24"/>
       <c r="J82" s="24"/>
@@ -2580,10 +2580,10 @@
       <c r="B83" s="24"/>
       <c r="C83" s="24"/>
       <c r="D83" s="24" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E83" s="24" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F83" s="24"/>
       <c r="G83" s="24"/>
@@ -2637,7 +2637,7 @@
         <v>114</v>
       </c>
       <c r="C89" t="s">
-        <v>319</v>
+        <v>345</v>
       </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.35">
@@ -2654,13 +2654,13 @@
         <v>27</v>
       </c>
       <c r="F91" t="s">
+        <v>145</v>
+      </c>
+      <c r="G91" t="s">
+        <v>147</v>
+      </c>
+      <c r="H91" t="s">
         <v>146</v>
-      </c>
-      <c r="G91" t="s">
-        <v>148</v>
-      </c>
-      <c r="H91" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.35">
@@ -2668,25 +2668,25 @@
         <v>114</v>
       </c>
       <c r="C92" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B93" s="27"/>
       <c r="D93" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E93" t="s">
         <v>73</v>
       </c>
       <c r="F93" t="s">
+        <v>149</v>
+      </c>
+      <c r="G93" t="s">
         <v>150</v>
       </c>
-      <c r="G93" t="s">
+      <c r="H93" t="s">
         <v>151</v>
-      </c>
-      <c r="H93" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.35">
@@ -2718,13 +2718,13 @@
         <v>27</v>
       </c>
       <c r="F98" t="s">
+        <v>152</v>
+      </c>
+      <c r="G98" t="s">
         <v>153</v>
       </c>
-      <c r="G98" t="s">
-        <v>154</v>
-      </c>
       <c r="H98" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.35">
@@ -2736,13 +2736,13 @@
         <v>65</v>
       </c>
       <c r="F99" t="s">
+        <v>154</v>
+      </c>
+      <c r="G99" t="s">
         <v>155</v>
       </c>
-      <c r="G99" t="s">
+      <c r="H99" t="s">
         <v>156</v>
-      </c>
-      <c r="H99" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.35">
@@ -2750,7 +2750,7 @@
         <v>114</v>
       </c>
       <c r="C100" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.35">
@@ -2762,13 +2762,13 @@
         <v>59</v>
       </c>
       <c r="F101" t="s">
+        <v>157</v>
+      </c>
+      <c r="G101" t="s">
         <v>158</v>
       </c>
-      <c r="G101" t="s">
-        <v>159</v>
-      </c>
       <c r="H101" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.35">
@@ -2793,16 +2793,16 @@
         <v>113</v>
       </c>
       <c r="E105" t="s">
+        <v>171</v>
+      </c>
+      <c r="F105" t="s">
+        <v>207</v>
+      </c>
+      <c r="G105" t="s">
         <v>172</v>
       </c>
-      <c r="F105" t="s">
-        <v>208</v>
-      </c>
-      <c r="G105" t="s">
+      <c r="H105" t="s">
         <v>173</v>
-      </c>
-      <c r="H105" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.35">
@@ -2815,7 +2815,7 @@
         <v>114</v>
       </c>
       <c r="C107" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="108" spans="1:12" x14ac:dyDescent="0.35">
@@ -2826,16 +2826,16 @@
     <row r="109" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B109" s="28"/>
       <c r="D109" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G109" t="s">
+        <v>275</v>
+      </c>
+      <c r="H109" t="s">
         <v>276</v>
       </c>
-      <c r="H109" t="s">
+      <c r="L109" t="s">
         <v>277</v>
-      </c>
-      <c r="L109" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.35">
@@ -2863,7 +2863,7 @@
         <v>114</v>
       </c>
       <c r="C114" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="115" spans="1:12" x14ac:dyDescent="0.35">
@@ -2873,21 +2873,21 @@
     </row>
     <row r="116" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D116" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G116" s="24" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H116" s="24" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="L116" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B118" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="119" spans="1:12" x14ac:dyDescent="0.35">
@@ -2920,52 +2920,52 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>220</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B2" t="s">
         <v>222</v>
-      </c>
-      <c r="B2" t="s">
-        <v>223</v>
       </c>
       <c r="C2" t="s">
         <v>112</v>
       </c>
       <c r="D2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>255</v>
+      </c>
+      <c r="B3" t="s">
+        <v>222</v>
+      </c>
+      <c r="C3" t="s">
+        <v>222</v>
+      </c>
+      <c r="D3" t="s">
         <v>256</v>
-      </c>
-      <c r="B3" t="s">
-        <v>223</v>
-      </c>
-      <c r="C3" t="s">
-        <v>223</v>
-      </c>
-      <c r="D3" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="18" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -2978,8 +2978,8 @@
   <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C69" sqref="C69"/>
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2998,7 +2998,7 @@
         <v>15</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>16</v>
@@ -3006,7 +3006,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B2" t="str">
         <f>"1"</f>
@@ -3021,7 +3021,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B3" t="str">
         <f>"2"</f>
@@ -3081,10 +3081,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B8" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C8" t="s">
         <v>32</v>
@@ -3095,10 +3095,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B9" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C9" t="s">
         <v>33</v>
@@ -3109,10 +3109,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B10" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C10" t="s">
         <v>34</v>
@@ -3123,10 +3123,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B11" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C11" t="s">
         <v>35</v>
@@ -3137,10 +3137,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B12" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C12" t="s">
         <v>36</v>
@@ -3151,10 +3151,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B13" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C13" t="s">
         <v>37</v>
@@ -3165,10 +3165,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B14" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C14" t="s">
         <v>38</v>
@@ -3179,10 +3179,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B15" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C15" t="s">
         <v>39</v>
@@ -3193,38 +3193,38 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B16" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C16" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D16" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B17" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B18" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C18" t="s">
         <v>40</v>
@@ -3235,72 +3235,72 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B19" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C19" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D19" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B20" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C20" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D20" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B21" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C21" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D21" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B22" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C22" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D22" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B23" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C23" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D23" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
@@ -3357,7 +3357,7 @@
         <v>4</v>
       </c>
       <c r="C30" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D30" t="s">
         <v>47</v>
@@ -3455,32 +3455,32 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B37" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D37" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B38" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
       <c r="C38" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
@@ -3567,10 +3567,10 @@
         <v>3</v>
       </c>
       <c r="C44" t="s">
+        <v>161</v>
+      </c>
+      <c r="D44" t="s">
         <v>162</v>
-      </c>
-      <c r="D44" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
@@ -3813,10 +3813,10 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B61" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C61" t="s">
         <v>29</v>
@@ -3827,82 +3827,82 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B62" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
       <c r="C62" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D62" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B63" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
       <c r="C63" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D63" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B64" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
       <c r="C64" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D64" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B65" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
       <c r="C65" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D65" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B66" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
       <c r="C66" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D66" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B67" t="str">
         <f>"3"</f>
@@ -3917,47 +3917,47 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B69" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
       <c r="C69" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D69" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B70" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
       <c r="C70" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D70" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B71" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
       <c r="C71" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D71" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
   </sheetData>
@@ -3989,248 +3989,248 @@
   <sheetData>
     <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="C1" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="D1" s="16" t="s">
         <v>179</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="E1" s="16" t="s">
         <v>180</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="F1" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="G1" s="16" t="s">
         <v>182</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="H1" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>184</v>
-      </c>
       <c r="I1" s="20" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E2" t="s">
+        <v>249</v>
+      </c>
+      <c r="F2" t="s">
         <v>250</v>
       </c>
-      <c r="F2" t="s">
-        <v>251</v>
-      </c>
       <c r="G2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E3" t="s">
+        <v>249</v>
+      </c>
+      <c r="F3" t="s">
         <v>250</v>
       </c>
-      <c r="F3" t="s">
-        <v>251</v>
-      </c>
       <c r="G3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>246</v>
+      </c>
+      <c r="B4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C4" t="s">
         <v>247</v>
       </c>
-      <c r="B4" t="s">
-        <v>175</v>
-      </c>
-      <c r="C4" t="s">
-        <v>248</v>
-      </c>
       <c r="D4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E4" t="s">
+        <v>249</v>
+      </c>
+      <c r="F4" t="s">
         <v>250</v>
       </c>
-      <c r="F4" t="s">
-        <v>251</v>
-      </c>
       <c r="G4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E5" t="s">
+        <v>249</v>
+      </c>
+      <c r="F5" t="s">
         <v>250</v>
       </c>
-      <c r="F5" t="s">
-        <v>251</v>
-      </c>
       <c r="G5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C7" t="s">
+        <v>248</v>
+      </c>
+      <c r="D7" t="s">
+        <v>248</v>
+      </c>
+      <c r="E7" t="s">
         <v>249</v>
       </c>
-      <c r="D7" t="s">
-        <v>249</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>250</v>
       </c>
-      <c r="F7" t="s">
-        <v>251</v>
-      </c>
       <c r="G7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="19" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E8" t="s">
+        <v>249</v>
+      </c>
+      <c r="F8" t="s">
         <v>250</v>
       </c>
-      <c r="F8" t="s">
-        <v>251</v>
-      </c>
       <c r="G8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="19" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E9" t="s">
+        <v>249</v>
+      </c>
+      <c r="F9" t="s">
         <v>250</v>
       </c>
-      <c r="F9" t="s">
-        <v>251</v>
-      </c>
       <c r="G9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="19" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C10" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D10" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E10" t="s">
+        <v>249</v>
+      </c>
+      <c r="F10" t="s">
         <v>250</v>
       </c>
-      <c r="F10" t="s">
-        <v>251</v>
-      </c>
       <c r="G10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -4242,9 +4242,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCD3AC6-97A9-4343-AD51-53B42E3E4B29}">
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4268,7 +4268,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B2" t="s">
         <v>113</v>
@@ -4279,10 +4279,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
@@ -4290,7 +4290,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B4" t="s">
         <v>113</v>
@@ -4301,10 +4301,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
@@ -4312,10 +4312,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B6" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C6" t="b">
         <v>0</v>
@@ -4323,7 +4323,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B7" t="s">
         <v>113</v>
@@ -4334,7 +4334,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>121</v>
+        <v>344</v>
       </c>
       <c r="B8" t="s">
         <v>113</v>
@@ -4345,7 +4345,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B9" t="s">
         <v>113</v>
@@ -4356,7 +4356,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B10" t="s">
         <v>113</v>
@@ -4368,10 +4368,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C11" t="b">
         <v>0</v>
@@ -4379,7 +4379,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B12" t="s">
         <v>113</v>
@@ -4390,7 +4390,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B13" t="s">
         <v>113</v>
@@ -4401,7 +4401,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B14" t="s">
         <v>113</v>
@@ -4415,7 +4415,7 @@
         <v>118</v>
       </c>
       <c r="B15" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C15" t="b">
         <v>0</v>
@@ -4423,10 +4423,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B16" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C16" t="b">
         <v>0</v>
@@ -4434,10 +4434,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C17" t="b">
         <v>1</v>
@@ -4445,7 +4445,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B18" t="s">
         <v>113</v>
@@ -4456,7 +4456,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B19" t="s">
         <v>113</v>
@@ -4467,10 +4467,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B20" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C20" t="b">
         <v>0</v>
@@ -4478,10 +4478,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B21" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C21" t="b">
         <v>0</v>
@@ -4489,7 +4489,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B22" t="s">
         <v>111</v>
@@ -4500,7 +4500,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B23" t="s">
         <v>113</v>
@@ -4511,7 +4511,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="24" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B24" s="24" t="s">
         <v>111</v>
@@ -4522,7 +4522,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B25" t="s">
         <v>113</v>
@@ -4533,7 +4533,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B26" t="s">
         <v>113</v>
@@ -4544,7 +4544,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B27" t="s">
         <v>113</v>
@@ -4555,7 +4555,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B28" t="s">
         <v>113</v>
@@ -4566,10 +4566,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C30" t="b">
         <v>0</v>
@@ -4577,10 +4577,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C31" t="b">
         <v>0</v>
@@ -4588,7 +4588,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B32" t="s">
         <v>113</v>
@@ -4599,7 +4599,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B33" t="s">
         <v>111</v>
@@ -4610,10 +4610,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B34" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C34" t="b">
         <v>0</v>
@@ -4621,10 +4621,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B35" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C35" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
updates to OOP tables
</commit_message>
<xml_diff>
--- a/app/config/tables/MIF_VISIT/forms/MIF_VISIT/MIF_VISIT.xlsx
+++ b/app/config/tables/MIF_VISIT/forms/MIF_VISIT/MIF_VISIT.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1245229B-031E-4005-B2C5-EC95D0DEBD50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71832317-DFE1-42A3-84C3-4DA8C89A2EF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -929,9 +929,6 @@
     <t>Gibril</t>
   </si>
   <si>
-    <t xml:space="preserve">Volar </t>
-  </si>
-  <si>
     <t xml:space="preserve">Isna </t>
   </si>
   <si>
@@ -1074,6 +1071,9 @@
   </si>
   <si>
     <t>data('GR') != '1' || (data('PARPAD') != '2' &amp;&amp; data('PARPAD3') != '1')</t>
+  </si>
+  <si>
+    <t>Voler</t>
   </si>
 </sst>
 </file>
@@ -1718,9 +1718,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F97EDFF-72E2-4781-A226-FCA8C7C63015}">
   <dimension ref="A1:L119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C100" sqref="C100"/>
+      <selection pane="bottomLeft" activeCell="C95" sqref="C95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1801,10 +1801,10 @@
         <v>113</v>
       </c>
       <c r="E4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G4" t="s">
         <v>121</v>
@@ -1922,7 +1922,7 @@
         <v>258</v>
       </c>
       <c r="H17" s="24" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="L17" t="s">
         <v>280</v>
@@ -1944,7 +1944,7 @@
         <v>114</v>
       </c>
       <c r="C21" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.35">
@@ -1958,10 +1958,10 @@
         <v>187</v>
       </c>
       <c r="G23" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H23" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.35">
@@ -1972,7 +1972,7 @@
         <v>27</v>
       </c>
       <c r="F24" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.35">
@@ -1991,7 +1991,7 @@
         <v>114</v>
       </c>
       <c r="C27" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.35">
@@ -2000,7 +2000,7 @@
         <v>114</v>
       </c>
       <c r="C28" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.35">
@@ -2014,10 +2014,10 @@
         <v>187</v>
       </c>
       <c r="G30" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H30" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.35">
@@ -2095,7 +2095,7 @@
         <v>114</v>
       </c>
       <c r="C37" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.35">
@@ -2109,10 +2109,10 @@
         <v>187</v>
       </c>
       <c r="G39" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="H39" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.35">
@@ -2190,7 +2190,7 @@
         <v>114</v>
       </c>
       <c r="C47" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.35">
@@ -2333,32 +2333,32 @@
         <v>194</v>
       </c>
       <c r="F61" t="s">
+        <v>322</v>
+      </c>
+      <c r="G61" t="s">
         <v>323</v>
       </c>
-      <c r="G61" t="s">
-        <v>324</v>
-      </c>
       <c r="H61" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" s="27"/>
       <c r="B62" s="5"/>
       <c r="D62" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E62" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F62" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G62" t="s">
+        <v>332</v>
+      </c>
+      <c r="H62" t="s">
         <v>333</v>
-      </c>
-      <c r="H62" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.35">
@@ -2637,7 +2637,7 @@
         <v>114</v>
       </c>
       <c r="C89" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.35">
@@ -2863,7 +2863,7 @@
         <v>114</v>
       </c>
       <c r="C114" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="115" spans="1:12" x14ac:dyDescent="0.35">
@@ -2977,9 +2977,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF3D0A7-17A8-4B35-89BF-E7F3088D1597}">
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A59" sqref="A59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3081,10 +3081,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B8" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C8" t="s">
         <v>32</v>
@@ -3095,10 +3095,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B9" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C9" t="s">
         <v>33</v>
@@ -3109,10 +3109,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B10" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C10" t="s">
         <v>34</v>
@@ -3123,10 +3123,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B11" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C11" t="s">
         <v>35</v>
@@ -3137,10 +3137,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C12" t="s">
         <v>36</v>
@@ -3151,10 +3151,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B13" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C13" t="s">
         <v>37</v>
@@ -3165,10 +3165,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B14" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C14" t="s">
         <v>38</v>
@@ -3179,10 +3179,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B15" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C15" t="s">
         <v>39</v>
@@ -3193,10 +3193,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B16" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C16" t="s">
         <v>293</v>
@@ -3207,10 +3207,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B17" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C17" t="s">
         <v>294</v>
@@ -3221,10 +3221,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B18" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C18" t="s">
         <v>40</v>
@@ -3235,10 +3235,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B19" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C19" t="s">
         <v>295</v>
@@ -3249,10 +3249,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B20" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C20" t="s">
         <v>296</v>
@@ -3263,44 +3263,44 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B21" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C21" t="s">
-        <v>297</v>
+        <v>345</v>
       </c>
       <c r="D21" t="s">
-        <v>297</v>
+        <v>345</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B22" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C22" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D22" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B23" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C23" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D23" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
@@ -3917,47 +3917,47 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B69" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
       <c r="C69" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D69" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B70" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
       <c r="C70" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D70" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B71" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
       <c r="C71" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D71" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
   </sheetData>
@@ -4301,7 +4301,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B5" t="s">
         <v>194</v>
@@ -4312,10 +4312,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B6" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C6" t="b">
         <v>0</v>
@@ -4334,7 +4334,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B8" t="s">
         <v>113</v>
@@ -4577,7 +4577,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B31" s="18" t="s">
         <v>194</v>
@@ -4588,7 +4588,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B32" t="s">
         <v>113</v>
@@ -4621,7 +4621,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B35" t="s">
         <v>194</v>

</xml_diff>